<commit_message>
Updates to incorporate Cambodian data
</commit_message>
<xml_diff>
--- a/agquery/Update/instrument_list.xlsx
+++ b/agquery/Update/instrument_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\New AgQ+ WD\AgQueryPlus\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2F485C-C757-454E-A7A0-B0D53B360341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474752FC-D587-4EF2-9682-7146AF21347E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="585" yWindow="690" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>survey</t>
   </si>
@@ -65,46 +65,28 @@
     <t>cons_ppp</t>
   </si>
   <si>
-    <t>GHS</t>
-  </si>
-  <si>
-    <t>nga</t>
-  </si>
-  <si>
-    <t>🇳🇬</t>
-  </si>
-  <si>
-    <t>w2</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>2012-13</t>
-  </si>
-  <si>
-    <t>w3</t>
-  </si>
-  <si>
-    <t>2015-16</t>
-  </si>
-  <si>
-    <t>w4</t>
-  </si>
-  <si>
-    <t>2018-19</t>
-  </si>
-  <si>
     <t>w1</t>
   </si>
   <si>
-    <t>2010-11</t>
-  </si>
-  <si>
     <t>gdp_ppp_2017</t>
   </si>
   <si>
     <t>cons_ppp_2017</t>
+  </si>
+  <si>
+    <t>CAS</t>
+  </si>
+  <si>
+    <t>khm</t>
+  </si>
+  <si>
+    <t>🇰🇭</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>2019-2020</t>
   </si>
 </sst>
 </file>
@@ -112,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -155,18 +137,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -484,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,33 +497,33 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1">
         <v>0.51738278250551617</v>
@@ -565,120 +538,6 @@
         <v>115.9778</v>
       </c>
       <c r="L2">
-        <v>112.0983276</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>2012</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0.62980571072215596</v>
-      </c>
-      <c r="I3">
-        <v>90.261179999999996</v>
-      </c>
-      <c r="J3">
-        <v>90.785850519999997</v>
-      </c>
-      <c r="K3">
-        <v>115.9778</v>
-      </c>
-      <c r="L3">
-        <v>112.0983276</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>2015</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.85819585393598818</v>
-      </c>
-      <c r="I4">
-        <v>105.37390000000001</v>
-      </c>
-      <c r="J4">
-        <v>101.90827179999999</v>
-      </c>
-      <c r="K4">
-        <v>115.9778</v>
-      </c>
-      <c r="L4">
-        <v>112.0983276</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5">
-        <v>2018</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1.2486994245960339</v>
-      </c>
-      <c r="I5">
-        <v>135.40199999999999</v>
-      </c>
-      <c r="J5">
-        <v>134.20745600000001</v>
-      </c>
-      <c r="K5">
-        <v>115.9778</v>
-      </c>
-      <c r="L5">
         <v>112.0983276</v>
       </c>
     </row>

</xml_diff>